<commit_message>
Add staging1 step to pipeline
</commit_message>
<xml_diff>
--- a/datanym/assets/IRS527/input_data/mappings.xlsx
+++ b/datanym/assets/IRS527/input_data/mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaac.flath/github/political-spending-analysis/DataConfigs/irs-fillings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaacflath/github/codenym/DataPipelines/datanym/assets/IRS527/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D44C9B1-7426-9745-BD19-9011E38D713B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0A75B1-C5F9-7245-8041-8D7045EFAD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14460" windowHeight="21900" xr2:uid="{49383944-EE1D-F149-B6E0-1A272E2D2BEE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="7" xr2:uid="{49383944-EE1D-F149-B6E0-1A272E2D2BEE}"/>
   </bookViews>
   <sheets>
     <sheet name="key" sheetId="8" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">E!$A$1:$D$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'R'!$A$1:$D$14</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,6 +43,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -332,30 +334,6 @@
   </si>
   <si>
     <t>SCHED B ID</t>
-  </si>
-  <si>
-    <t>RECIEPIENT NAME</t>
-  </si>
-  <si>
-    <t>RECIEPIENT ADDRESS 1</t>
-  </si>
-  <si>
-    <t>RECIEPIENT ADDRESS 2</t>
-  </si>
-  <si>
-    <t>RECIEPIENT ADDRESS CITY</t>
-  </si>
-  <si>
-    <t>RECIEPIENT ADDRESS ST</t>
-  </si>
-  <si>
-    <t>RECIEPIENT ADDRESS ZIP CODE</t>
-  </si>
-  <si>
-    <t>RECIEPIENT ADDRESS ZIP EXT</t>
-  </si>
-  <si>
-    <t>RECIEPIENT EMPLOYER</t>
   </si>
   <si>
     <t>EXPENDITURE AMOUNT</t>
@@ -436,6 +414,30 @@
   </si>
   <si>
     <t>If a Schedule B exists for an 8872 Form, each Schedule B record will be printed out in an “B” record.  The “B” records for a given 8872 Form will follow its related “2” Record.  There may be several “B” records for any one “2” record.</t>
+  </si>
+  <si>
+    <t>RECIPIENT NAME</t>
+  </si>
+  <si>
+    <t>RECIPIENT ADDRESS 1</t>
+  </si>
+  <si>
+    <t>RECIPIENT ADDRESS 2</t>
+  </si>
+  <si>
+    <t>RECIPIENT ADDRESS CITY</t>
+  </si>
+  <si>
+    <t>RECIPIENT ADDRESS ZIP CODE</t>
+  </si>
+  <si>
+    <t>RECIPIENT ADDRESS ZIP EXT</t>
+  </si>
+  <si>
+    <t>RECIPIENT EMPLOYER</t>
+  </si>
+  <si>
+    <t>RECIPIENT ADDRESS STATE</t>
   </si>
 </sst>
 </file>
@@ -489,16 +491,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -821,7 +822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E7E947-AE86-DC47-81DE-5BAF3EF3C10C}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
@@ -829,87 +830,87 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>118</v>
+        <v>103</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>119</v>
+        <v>101</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>120</v>
+        <v>105</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
-        <v>115</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>121</v>
+        <v>107</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D6" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>122</v>
+      <c r="D6" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>123</v>
+        <v>108</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>92</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>124</v>
+      <c r="E8" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -927,684 +928,683 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="str">
+      <c r="A2" t="str">
         <f>SUBSTITUTE(LOWER(B2)," ","_")</f>
         <v>record_type</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="str">
+      <c r="A3" t="str">
         <f t="shared" ref="A3:A45" si="0">SUBSTITUTE(LOWER(B3)," ","_")</f>
         <v>form_type</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="str">
+      <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>form_id_number</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="str">
+      <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>initial_report_indicator</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="str">
+      <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>amended_report_indicator</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="str">
+      <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>final_report_indicator</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="str">
+      <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>ein</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="str">
+      <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>organization_name</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="C9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="str">
+      <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>mailing_address_1</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="C10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="str">
+      <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>mailing_address_2</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="C11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="str">
+      <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>mailing_address_city</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="C12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="str">
+      <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>mailing_address_state</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="str">
+      <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>mailing_address_zip_code</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="C14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="str">
+      <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>mailing_address_zip_ext</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="C15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="str">
+      <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>e_mail_address</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="C16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="str">
+      <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>established_date</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="C17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="str">
+      <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>custodian_name</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="C18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="str">
+      <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>custodian_address_1</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" s="1">
+      <c r="C19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="str">
+      <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>custodian_address_2</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="C20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="str">
+      <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>custodian_address_city</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="1">
+      <c r="C21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="str">
+      <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>custodian_address_state</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D22" s="1">
+      <c r="C22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="str">
+      <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>custodian_address_zip_code</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D23" s="1">
+      <c r="C23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="str">
+      <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>custodian_address_zip_ext</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" s="1">
+      <c r="C24" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="str">
+      <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>contact_person_name</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D25" s="1">
+      <c r="C25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="str">
+      <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>contact_address_1</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="1">
+      <c r="C26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="str">
+      <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>contact_address_2</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="1">
+      <c r="C27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="str">
+      <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>contact_address_city</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" s="1">
+      <c r="C28" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="str">
+      <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>contact_address_state</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" s="1">
+      <c r="C29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="str">
+      <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>contact_address_zip_code</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D30" s="1">
+      <c r="C30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="str">
+      <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>contact_address_zip_ext</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D31" s="1">
+      <c r="C31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="str">
+      <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>business_address_1</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D32" s="1">
+      <c r="C32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="str">
+      <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>business_address_2</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="1">
+      <c r="C33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="str">
+      <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>business_address_city</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D34" s="1">
+      <c r="C34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="str">
+      <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>business_address_state</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D35" s="1">
+      <c r="C35" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="str">
+      <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>business_address_zip_code</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D36" s="1">
+      <c r="C36" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="str">
+      <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>business_address_zip_ext</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" s="1">
+      <c r="C37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="str">
+      <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>exempt_8872_indicator</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D38" s="1">
+      <c r="C38" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="str">
+      <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>exempt_state</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D39" s="1">
+      <c r="C39" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39">
         <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="str">
+      <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>exempt_990_indicator</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D40" s="1">
+      <c r="C40" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40">
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="str">
+      <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>purpose</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D41" s="1">
+      <c r="C41" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="str">
+      <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>material_change_date</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D42" s="1">
+      <c r="C42" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="str">
+      <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>insert_datetime</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D43" s="1">
+      <c r="C43" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43">
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="str">
+      <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>related_entity_bypass</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D44" s="1">
+      <c r="C44" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D44">
         <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="str">
+      <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>eain_bypass</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D45" s="1">
+      <c r="C45" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45">
         <v>43</v>
       </c>
     </row>
@@ -1623,219 +1623,218 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="str">
+      <c r="A2" t="str">
         <f t="shared" ref="A2:A14" si="0">SUBSTITUTE(LOWER(B2)," ","_")</f>
         <v>record_type</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="str">
+      <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>form_id_number</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="str">
+      <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>director_id</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="str">
+      <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>org_name</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="str">
+      <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>ein</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="str">
+      <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>entity_name</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="str">
+      <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>entity_title</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="str">
+      <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>entity_address_1</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="C9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="str">
+      <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>entity_address_2</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="C10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="str">
+      <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>entity_address_city</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="C11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="str">
+      <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>entity_address_st</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="C12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="str">
+      <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>entity_address_zip_code</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="str">
+      <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>entity_address_zip_code_ext</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="C14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14">
         <v>12</v>
       </c>
     </row>
@@ -1854,219 +1853,218 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="str">
+      <c r="A2" t="str">
         <f t="shared" ref="A2:A14" si="0">SUBSTITUTE(LOWER(B2)," ","_")</f>
         <v>record_type</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="str">
+      <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>form_id_number</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="str">
+      <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>entity_id</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="str">
+      <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>org_name</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="str">
+      <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>ein</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="str">
+      <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>entity_name</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="str">
+      <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>entity_relationship</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="str">
+      <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>entity_address_1</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="C9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="str">
+      <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>entity_address_2</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="C10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="str">
+      <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>entity_address_city</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="C11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="str">
+      <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>entity_address_st</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="C12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="str">
+      <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>entity_address_zip_code</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="str">
+      <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>entity_address_zip_ext</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="C14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14">
         <v>12</v>
       </c>
     </row>
@@ -2085,99 +2083,98 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="str">
+      <c r="A2" t="str">
         <f t="shared" ref="A2:A6" si="0">SUBSTITUTE(LOWER(B2)," ","_")</f>
         <v>record_type</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="str">
+      <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>form_id_number</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="str">
+      <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>eain_id</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="str">
+      <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>election_authority_id_number</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="str">
+      <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>state_issued</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6">
         <v>4</v>
       </c>
     </row>
@@ -2196,759 +2193,758 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="str">
+      <c r="A2" t="str">
         <f t="shared" ref="A2:A50" si="0">SUBSTITUTE(LOWER(B2)," ","_")</f>
         <v>record_type</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="str">
+      <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>form_type</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="str">
+      <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>form_id_number</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="str">
+      <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>period_begin_date</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="str">
+      <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>period_end_date</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="str">
+      <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>initial_report_indicator</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="str">
+      <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>amended_report_indicator</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="str">
+      <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>final_report_indicator</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="C9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="str">
+      <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>change_of_address_indicator</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="C10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="str">
+      <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>organization_name</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="C11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="str">
+      <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>ein</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="C12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="str">
+      <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>mailing_address_1</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="str">
+      <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>mailing_address_2</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="C14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="str">
+      <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>mailing_address_city</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="C15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="str">
+      <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>mailing_address_state</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="C16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="str">
+      <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>mailing_address_zip_code</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="C17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="str">
+      <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>mailing_address_zip_ext</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="C18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="str">
+      <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>e_mail_address</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" s="1">
+      <c r="C19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="str">
+      <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>org_formation_date</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="C20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="str">
+      <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>custodian_name</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="1">
+      <c r="C21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="str">
+      <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>custodian_address_1</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D22" s="1">
+      <c r="C22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="str">
+      <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>custodian_address_2</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D23" s="1">
+      <c r="C23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="str">
+      <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>custodian_address_city</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" s="1">
+      <c r="C24" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="str">
+      <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>custodian_address_state</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D25" s="1">
+      <c r="C25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="str">
+      <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>custodian_address_zip_code</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D26" s="1">
+      <c r="C26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="str">
+      <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>custodian_address_zip_ext</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="1">
+      <c r="C27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="str">
+      <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>contact_person_name</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" s="1">
+      <c r="C28" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="str">
+      <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>contact_address_1</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" s="1">
+      <c r="C29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="str">
+      <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>contact_address_2</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D30" s="1">
+      <c r="C30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="str">
+      <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>contact_address_city</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D31" s="1">
+      <c r="C31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="str">
+      <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>contact_address_state</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D32" s="1">
+      <c r="C32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="str">
+      <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>contact_address_zip_code</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="1">
+      <c r="C33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="str">
+      <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>contact_address_zip_ext</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D34" s="1">
+      <c r="C34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="str">
+      <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>business_address_1</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D35" s="1">
+      <c r="C35" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="str">
+      <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>business_address_2</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D36" s="1">
+      <c r="C36" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="str">
+      <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>business_address_city</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D37" s="1">
+      <c r="C37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="str">
+      <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>business_address_state</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D38" s="1">
+      <c r="C38" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38">
         <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="str">
+      <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>business_address_zip_code</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D39" s="1">
+      <c r="C39" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39">
         <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="str">
+      <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>business_address_zip_ext</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D40" s="1">
+      <c r="C40" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40">
         <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="str">
+      <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>qtr_indicator</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D41" s="1">
+      <c r="C41" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="str">
+      <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>monthly_rpt_month</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D42" s="1">
+      <c r="C42" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="str">
+      <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>pre_elect_type</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D43" s="1">
+      <c r="C43" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D43">
         <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="str">
+      <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>pre_or_post_elect_date</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D44" s="1">
+      <c r="C44" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D44">
         <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="str">
+      <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>pre_or_post_elect_state</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D45" s="1">
+      <c r="C45" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45">
         <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="str">
+      <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>sched_a_ind</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D46" s="1">
+      <c r="C46" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46">
         <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="str">
+      <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>total_sched_a</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D47" s="1">
+      <c r="C47" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D47">
         <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="str">
+      <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>sched_b_ind</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D48" s="1">
+      <c r="C48" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48">
         <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="str">
+      <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>total_sched_b</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D49" s="1">
+      <c r="C49" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49">
         <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="str">
+      <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>insert_datetime</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50" s="1">
+      <c r="C50" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50">
         <v>48</v>
       </c>
     </row>
@@ -2967,279 +2963,278 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="str">
+      <c r="A2" t="str">
         <f t="shared" ref="A2:A18" si="0">SUBSTITUTE(LOWER(B2)," ","_")</f>
         <v>record_type</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="str">
+      <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>form_id_number</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="str">
+      <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>sched_a_id</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="str">
+      <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>org_name</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="str">
+      <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>ein</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="str">
+      <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>contributor_name</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="str">
+      <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>contributor_address_1</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="str">
+      <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>contributor_address_2</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="C9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="str">
+      <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>contributor_address_city</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="C10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="str">
+      <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>contributor_address_state</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="C11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="str">
+      <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>contributor_address_zip_code</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="C12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="str">
+      <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>contributor_address_zip_ext</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="str">
+      <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>contributor_employer</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="C14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="str">
+      <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>contribution_amount</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="C15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="str">
+      <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>contributor_occupation</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="C16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="str">
+      <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>agg_contribution_ytd</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="C17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="str">
+      <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>contribution_date</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="C18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18">
         <v>16</v>
       </c>
     </row>
@@ -3252,285 +3247,284 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{969DCC60-D198-D041-B6EE-8132B1D30125}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="str">
+      <c r="A2" t="str">
         <f t="shared" ref="A2:A18" si="0">SUBSTITUTE(LOWER(B2)," ","_")</f>
         <v>record_type</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="str">
+      <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>form_id_number</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="str">
+      <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>sched_b_id</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="str">
+      <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>org_name</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="str">
+      <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>ein</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>reciepient_name</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>recipient_name</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>recipient_address_1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>recipient_address_2</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>recipient_address_city</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>recipient_address_state</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>recipient_address_zip_code</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>recipient_address_zip_ext</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>recipient_employer</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>expenditure_amount</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>reciepient_address_1</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>recipient_occupation</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>reciepient_address_2</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>expenditure_date</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>reciepient_address_city</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>expenditure_purpose</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>reciepient_address_st</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>reciepient_address_zip_code</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>reciepient_address_zip_ext</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>reciepient_employer</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>expenditure_amount</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>recipient_occupation</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>expenditure_date</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>expenditure_purpose</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="C18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18">
         <v>16</v>
       </c>
     </row>

</xml_diff>